<commit_message>
0702pm0555 added intro section to index.html
</commit_message>
<xml_diff>
--- a/reference/presentationNotes.xlsx
+++ b/reference/presentationNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorig\Documents\_GeorgiaTech\VizProj\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CB54B3-1FF1-4B39-B01A-965CF5D37D1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D93110E-8CF6-4E8B-8DAC-4A5872F46706}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5A5BAABA-E720-43E6-8C7B-08E31CC24CB3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A5BAABA-E720-43E6-8C7B-08E31CC24CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -351,8 +351,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -390,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,32 +402,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,17 +743,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242289A7-358A-4D5D-ADCC-35F6B5619934}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" customWidth="1"/>
     <col min="2" max="2" width="7.21875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="31" customWidth="1"/>
     <col min="4" max="4" width="61.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
@@ -772,19 +775,19 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="29" t="s">
@@ -810,7 +813,7 @@
       <c r="B6" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
@@ -824,7 +827,7 @@
       <c r="B7" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="31" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -842,7 +845,7 @@
       <c r="B8" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -880,7 +883,7 @@
       <c r="B10" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="17"/>
@@ -896,7 +899,7 @@
       <c r="B11" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -911,7 +914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="10">
         <v>1.0416666666666666E-2</v>
@@ -933,7 +936,7 @@
       <c r="B13" s="14">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="15" t="s">
         <v>14</v>
       </c>
@@ -945,7 +948,7 @@
     <row r="14" spans="1:8" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
-      <c r="C14" s="34"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="20" t="s">
         <v>17</v>
       </c>
@@ -959,7 +962,7 @@
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="34"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
@@ -973,7 +976,7 @@
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="34"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="20" t="s">
         <v>19</v>
       </c>
@@ -984,10 +987,10 @@
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
     </row>
-    <row r="17" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="73.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
       <c r="B17" s="24"/>
-      <c r="C17" s="35"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="25" t="s">
         <v>20</v>
       </c>
@@ -1018,7 +1021,7 @@
       <c r="B19" s="14">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C19" s="32"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="15" t="s">
         <v>25</v>
       </c>
@@ -1144,6 +1147,6 @@
     <mergeCell ref="E4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>